<commit_message>
convert distributions and treatment parsers to classes
</commit_message>
<xml_diff>
--- a/bio_diversity/static/data_templates/coldbrook-treatment.xlsx
+++ b/bio_diversity/static/data_templates/coldbrook-treatment.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Ponds" sheetId="1" r:id="rId1"/>
@@ -25,16 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="15">
-  <si>
-    <t>Stock 1</t>
-  </si>
-  <si>
-    <t>Stock 2</t>
-  </si>
-  <si>
-    <t>Stock 3</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="12">
   <si>
     <t>Treatment Type</t>
   </si>
@@ -444,55 +435,50 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:M4"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.28515625" customWidth="1"/>
-    <col min="8" max="8" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.7109375" customWidth="1"/>
-    <col min="10" max="10" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.42578125" customWidth="1"/>
+    <col min="7" max="7" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="51" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="4"/>
       <c r="J2" s="1"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="4"/>
-      <c r="M2" s="1"/>
     </row>
-    <row r="3" spans="1:13" ht="51" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="6" t="s">
         <v>8</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>11</v>
       </c>
       <c r="E3" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="7" t="s">
         <v>1</v>
       </c>
       <c r="G3" s="6" t="s">
@@ -501,33 +487,21 @@
       <c r="H3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="I3" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="J3" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="K3" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="L3" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="M3" s="5" t="s">
-        <v>14</v>
+      <c r="I3" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
+      <c r="H4" s="2"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="1"/>
-      <c r="M4" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -537,55 +511,49 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:M4"/>
+  <dimension ref="A2:J4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.140625" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" customWidth="1"/>
-    <col min="7" max="7" width="10.5703125" customWidth="1"/>
-    <col min="8" max="8" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.5703125" customWidth="1"/>
-    <col min="10" max="10" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.5703125" customWidth="1"/>
+    <col min="7" max="7" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
+      <c r="H2" s="3"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
     </row>
-    <row r="3" spans="1:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="6" t="s">
         <v>7</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>10</v>
       </c>
       <c r="E3" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="7" t="s">
         <v>1</v>
       </c>
       <c r="G3" s="6" t="s">
@@ -594,33 +562,21 @@
       <c r="H3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="I3" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="J3" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="K3" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="L3" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="M3" s="5" t="s">
-        <v>14</v>
+      <c r="I3" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
+      <c r="H4" s="3"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
-      <c r="K4" s="3"/>
-      <c r="L4" s="1"/>
-      <c r="M4" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fix small typos in templates and views
</commit_message>
<xml_diff>
--- a/bio_diversity/static/data_templates/coldbrook-treatment.xlsx
+++ b/bio_diversity/static/data_templates/coldbrook-treatment.xlsx
@@ -281,7 +281,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="14">
   <si>
     <t>Treatment Type</t>
   </si>
@@ -320,6 +320,9 @@
   </si>
   <si>
     <t>Water Level During Treatment (Inches)</t>
+  </si>
+  <si>
+    <t>Amount (Gal)</t>
   </si>
 </sst>
 </file>
@@ -709,7 +712,7 @@
   <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -757,7 +760,7 @@
         <v>12</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="H3" s="7" t="s">
         <v>11</v>

</xml_diff>